<commit_message>
5G and 4G Model
</commit_message>
<xml_diff>
--- a/validation/capacity model.xlsx
+++ b/validation/capacity model.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10908"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bosoro/Documents/GitHub/geosafi-consav/validation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27B8EE4D-3312-0B4A-8789-F564B15BC3E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D37207FF-90B5-0D49-A73A-69756DA6AFFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="42100" yWindow="500" windowWidth="32620" windowHeight="19540" xr2:uid="{923C292A-059E-F749-AE68-76132D262AD5}"/>
+    <workbookView xWindow="5600" yWindow="6960" windowWidth="36060" windowHeight="22320" xr2:uid="{923C292A-059E-F749-AE68-76132D262AD5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="LTE" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="74">
   <si>
     <t>Parameter</t>
   </si>
@@ -204,13 +205,67 @@
   </si>
   <si>
     <t>Hata Okamura Path Loss (Rural Areas)</t>
+  </si>
+  <si>
+    <t>30-50</t>
+  </si>
+  <si>
+    <t>1.5 - 10</t>
+  </si>
+  <si>
+    <t>1/K</t>
+  </si>
+  <si>
+    <t>K = Number of cells</t>
+  </si>
+  <si>
+    <t>Handoff factor</t>
+  </si>
+  <si>
+    <t>Antenna Noise - AWGN</t>
+  </si>
+  <si>
+    <t>Set noise floor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SNR Threshold </t>
+  </si>
+  <si>
+    <t>16-23</t>
+  </si>
+  <si>
+    <t>0-3</t>
+  </si>
+  <si>
+    <t>4G</t>
+  </si>
+  <si>
+    <t>System Temperature</t>
+  </si>
+  <si>
+    <t>k</t>
+  </si>
+  <si>
+    <t>Multiple Access Scheme</t>
+  </si>
+  <si>
+    <t>700/1800</t>
+  </si>
+  <si>
+    <t>JTL given 700 MHz in Kenya</t>
+  </si>
+  <si>
+    <t>TDD/OFDMA/SCDMA</t>
+  </si>
+  <si>
+    <t>SCDMA - UL and OFDMA - DL to achieve max. peak to average power ratio</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -233,8 +288,15 @@
       <family val="2"/>
       <scheme val="major"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF00B050"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -253,8 +315,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -277,17 +345,51 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -604,8 +706,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83D24FE3-A951-E44C-A5F6-DCACE8A449BF}">
   <dimension ref="A1:H22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="139" zoomScaleNormal="139" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView tabSelected="1" zoomScale="185" zoomScaleNormal="185" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1015,4 +1117,289 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0C8DDBD-578E-7A42-9DE5-7C7F817DB3C2}">
+  <dimension ref="A1:E27"/>
+  <sheetViews>
+    <sheetView zoomScale="209" zoomScaleNormal="209" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="32.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="3">
+        <v>20</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="3">
+        <v>1</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D6" t="s">
+        <v>58</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="3">
+        <v>40</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" s="3">
+        <v>3</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B14" s="3">
+        <v>4</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B15" s="3">
+        <v>4</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B17" s="3">
+        <v>294</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B18" s="3">
+        <v>50</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="C19" s="3"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B20" s="3">
+        <v>20</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24" s="7" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25" s="7" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26" s="7" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A27" s="7" t="s">
+        <v>73</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:C1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>